<commit_message>
Update portfolio data and analytics: Add comprehensive reports, validation scripts, and property-level analysis
- Add comprehensive portfolio reports and calculation standards compliance
- Add multiple Python utilities for report generation and validation
- Update WasteWise analytics with validated data
- Add property-specific expense reports and regulatory analysis
- Reorganize invoice files from The Club at Millenia to Bella Mirage
- Update master portfolio data and property reference sheets
- Add vendor name mapping and property configuration files
</commit_message>
<xml_diff>
--- a/Portfolio_Reports/MASTER_Portfolio_Complete_Data.xlsx
+++ b/Portfolio_Reports/MASTER_Portfolio_Complete_Data.xlsx
@@ -69638,7 +69638,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Garden Style</t>
+          <t>8x 8YD + 2x 10YD</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -69686,16 +69686,16 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>8 YD</t>
+          <t>30 YD</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>4x/week</t>
+          <t>On-call (varies)</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -69721,12 +69721,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Compactor</t>
+          <t>Dumpster</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Garden Style</t>
+          <t>Mixed (8YD, 6YD, 4YD)</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -69739,7 +69739,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3x/week</t>
+          <t>4x/week</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -69774,16 +69774,16 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>40 CY</t>
+          <t>30 CY</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2.4x/week (on-call)</t>
+          <t>On-call (2-3x/week)</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -69809,7 +69809,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Compactor</t>
+          <t>Dumpster</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -69941,16 +69941,16 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Mixed</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Garden Style</t>
+          <t>Mixed (3YD, 4YD)</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -69959,7 +69959,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>3x/week</t>
+          <t>1x-3x/week</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -70340,7 +70340,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
@@ -70393,14 +70393,14 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>67324.17</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>7534.366672058823</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>10.53757576511724</v>
+      <c r="C2" t="n">
+        <v>65924.17</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6592.416999999999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>92.20163636363637</v>
       </c>
     </row>
     <row r="3">
@@ -70414,14 +70414,14 @@
           <t>extra_pickup</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>33813.83</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>3784.165386764706</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>5.29253900246812</v>
+      <c r="C3" t="n">
+        <v>980</v>
+      </c>
+      <c r="D3" t="n">
+        <v>98</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.370629370629371</v>
       </c>
     </row>
     <row r="4">
@@ -70435,14 +70435,14 @@
           <t>overage</t>
         </is>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>20171.6</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>2257.439352941176</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>3.157257836281365</v>
+      <c r="C4" t="n">
+        <v>420</v>
+      </c>
+      <c r="D4" t="n">
+        <v>42</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.5874125874125874</v>
       </c>
     </row>
     <row r="5">
@@ -70456,14 +70456,14 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>99156.67999999999</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>11056.15142564103</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>26.57728708086785</v>
+      <c r="C5" t="n">
+        <v>91515.45000000001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10168.38333333334</v>
+      </c>
+      <c r="E5" t="n">
+        <v>219.9890625</v>
       </c>
     </row>
     <row r="6">
@@ -70477,14 +70477,14 @@
           <t>extra_pickup</t>
         </is>
       </c>
-      <c r="C6" s="5" t="n">
-        <v>11279.6</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>1257.696058608059</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>3.023307833192449</v>
+      <c r="C6" t="n">
+        <v>86.25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.583333333333334</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2073317307692308</v>
       </c>
     </row>
     <row r="7">
@@ -70498,14 +70498,14 @@
           <t>tax</t>
         </is>
       </c>
-      <c r="C7" s="5" t="n">
-        <v>99156.67999999999</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>11056.15142564103</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>26.57728708086785</v>
+      <c r="C7" t="n">
+        <v>7556.98</v>
+      </c>
+      <c r="D7" t="n">
+        <v>839.6644444444444</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18.16581730769231</v>
       </c>
     </row>
     <row r="8">
@@ -70519,14 +70519,14 @@
           <t>admin</t>
         </is>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>54439.09</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>6819.448146502059</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>15.05396941832684</v>
+      <c r="C8" t="n">
+        <v>39</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.08609271523178808</v>
       </c>
     </row>
     <row r="9">
@@ -70540,14 +70540,14 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C9" s="5" t="n">
-        <v>57064.64</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>7148.344204115227</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>15.78000928060756</v>
+      <c r="C9" t="n">
+        <v>53420.55999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3561.370666666666</v>
+      </c>
+      <c r="E9" t="n">
+        <v>117.9261810154525</v>
       </c>
     </row>
     <row r="10">
@@ -70561,14 +70561,14 @@
           <t>franchise_fee</t>
         </is>
       </c>
-      <c r="C10" s="5" t="n">
-        <v>54666.45</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>6847.928962962964</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>15.11684097784319</v>
+      <c r="C10" t="n">
+        <v>1405.51</v>
+      </c>
+      <c r="D10" t="n">
+        <v>93.70066666666665</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.102671081677704</v>
       </c>
     </row>
     <row r="11">
@@ -70582,14 +70582,14 @@
           <t>overage</t>
         </is>
       </c>
-      <c r="C11" s="5" t="n">
-        <v>227.36</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>28.48081646090535</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>0.06287155951634731</v>
+      <c r="C11" t="n">
+        <v>200</v>
+      </c>
+      <c r="D11" t="n">
+        <v>13.33333333333333</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4415011037527594</v>
       </c>
     </row>
     <row r="12">
@@ -70603,14 +70603,14 @@
           <t>tax</t>
         </is>
       </c>
-      <c r="C12" s="5" t="n">
-        <v>57292</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>7176.825020576132</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>15.84288084012391</v>
+      <c r="C12" t="n">
+        <v>4157.78</v>
+      </c>
+      <c r="D12" t="n">
+        <v>277.1853333333333</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9.178322295805739</v>
       </c>
     </row>
     <row r="13">
@@ -70624,14 +70624,14 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C13" s="5" t="n">
-        <v>34478.73</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>4950.625194339624</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>15.86738844339623</v>
+      <c r="C13" t="n">
+        <v>29890.44</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3736.305</v>
+      </c>
+      <c r="E13" t="n">
+        <v>95.80269230769231</v>
       </c>
     </row>
     <row r="14">
@@ -70645,14 +70645,14 @@
           <t>other</t>
         </is>
       </c>
-      <c r="C14" s="5" t="n">
-        <v>3959.88</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>568.5789962264151</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>1.822368577648766</v>
+      <c r="C14" t="n">
+        <v>-4278.17</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-534.77125</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-13.71208333333333</v>
       </c>
     </row>
     <row r="15">
@@ -70666,14 +70666,14 @@
           <t>overage</t>
         </is>
       </c>
-      <c r="C15" s="5" t="n">
-        <v>33173.92</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>4763.274173584906</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>15.26690440251572</v>
+      <c r="C15" t="n">
+        <v>1960.4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>245.05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6.283333333333332</v>
       </c>
     </row>
     <row r="16">
@@ -70687,14 +70687,14 @@
           <t>tax</t>
         </is>
       </c>
-      <c r="C16" s="5" t="n">
-        <v>34478.73</v>
-      </c>
-      <c r="D16" s="5" t="n">
-        <v>4950.625194339624</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>15.86738844339623</v>
+      <c r="C16" t="n">
+        <v>2627.89</v>
+      </c>
+      <c r="D16" t="n">
+        <v>328.48625</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8.42272435897436</v>
       </c>
     </row>
     <row r="17">
@@ -70708,14 +70708,14 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C17" s="5" t="n">
-        <v>31168.6</v>
-      </c>
-      <c r="D17" s="5" t="n">
-        <v>5241.835270718232</v>
-      </c>
-      <c r="E17" s="5" t="n">
-        <v>17.0189456841501</v>
+      <c r="C17" t="n">
+        <v>18909.69</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2363.71125</v>
+      </c>
+      <c r="E17" t="n">
+        <v>61.39509740259741</v>
       </c>
     </row>
     <row r="18">
@@ -70729,14 +70729,14 @@
           <t>extra_pickup</t>
         </is>
       </c>
-      <c r="C18" s="5" t="n">
-        <v>12630.86</v>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>2124.217560220995</v>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v>6.896810260457775</v>
+      <c r="C18" t="n">
+        <v>6871.800000000002</v>
+      </c>
+      <c r="D18" t="n">
+        <v>858.9750000000003</v>
+      </c>
+      <c r="E18" t="n">
+        <v>22.31103896103897</v>
       </c>
     </row>
     <row r="19">
@@ -70750,14 +70750,14 @@
           <t>other</t>
         </is>
       </c>
-      <c r="C19" s="5" t="n">
-        <v>8044.36</v>
-      </c>
-      <c r="D19" s="5" t="n">
-        <v>1352.874687292817</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>4.392450283418239</v>
+      <c r="C19" t="n">
+        <v>-7101.410000000001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-887.6762500000001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-23.05652597402598</v>
       </c>
     </row>
     <row r="20">
@@ -70771,182 +70771,14 @@
           <t>tax</t>
         </is>
       </c>
-      <c r="C20" s="5" t="n">
-        <v>31168.6</v>
-      </c>
-      <c r="D20" s="5" t="n">
-        <v>5241.835270718232</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>17.0189456841501</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>The Club at Millenia</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Container Rental</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>10234.8</v>
-      </c>
-      <c r="D21" s="5" t="n">
-        <v>2036.25694117647</v>
-      </c>
-      <c r="E21" s="5" t="n">
-        <v>3.636173109243698</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>The Club at Millenia</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Bulk/Extra Pickups</t>
-        </is>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>6414.24</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>1276.140298039216</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>2.278821960784314</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>The Club at Millenia</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Other Services</t>
-        </is>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>27387.16</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>5448.791832679741</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>9.729985415499531</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>The Club at Millenia</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Disposal</t>
-        </is>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>26024.96</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>5177.776355555556</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>9.246029206349206</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Mandarina</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>General Waste Service</t>
-        </is>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>34460.72</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <v>2997.098048</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>16.65054471111111</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Pavilions at Arrowhead</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>General Waste Service</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>42323.46000000001</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>3845.749619104478</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>15.50705491574386</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Springs at Alta Mesa</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>General Waste Service</t>
-        </is>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>192171.15</v>
-      </c>
-      <c r="D27" s="5" t="n">
-        <v>17461.76061492537</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>87.30880307462687</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Tempe Vista</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>General Waste Service</t>
-        </is>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>33738.18</v>
-      </c>
-      <c r="D28" s="5" t="n">
-        <v>3074.820955688623</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>16.53129546069152</v>
+      <c r="C20" t="n">
+        <v>2136.09</v>
+      </c>
+      <c r="D20" t="n">
+        <v>267.01125</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6.935357142857144</v>
       </c>
     </row>
   </sheetData>
@@ -70960,7 +70792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -71011,45 +70843,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tempe Vista</t>
+          <t>Bella Mirage</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4 yards</t>
+          <t>8 YD</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>4x/week</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tempe Vista</t>
+          <t>Bella Mirage</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6 yards</t>
+          <t>6 YD</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -71057,7 +70889,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>4x/week</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -71067,17 +70899,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tempe Vista</t>
+          <t>Bella Mirage</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8 yards</t>
+          <t>4 YD</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -71085,11 +70917,11 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>4x/week</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -71105,7 +70937,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6 yards</t>
+          <t>6 YD</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -71113,7 +70945,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>3x/week</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -71123,136 +70955,141 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Springs at Alta Mesa</t>
+          <t>McCord Park FL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6 yards</t>
+          <t>8 YD</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>3x/week</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Springs at Alta Mesa</t>
+          <t>Orion McKinney</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4 yards</t>
+          <t>10 YD</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>3x/week</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Springs at Alta Mesa</t>
+          <t>Orion McKinney</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cart</t>
+          <t>Dumpster (FEL)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>90 gallons</t>
+          <t>8 YD</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3x per week</t>
+          <t>3x/week</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Springs at Alta Mesa</t>
+          <t>Orion Prosper</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bulk</t>
+          <t>Compactor</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10 YD</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Weekly (Thursday)</t>
+          <t>6x/week</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pavilions at Arrowhead</t>
+          <t>Orion Prosper Lakes</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dumpster</t>
+          <t>Compactor</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4 yards</t>
+          <t>30 CY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2x per week</t>
+          <t>On-call (2-3x/week avg)</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -71263,7 +71100,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bulk</t>
+          <t>Bulk Service</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -71276,6 +71113,253 @@
       </c>
       <c r="F11" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Pavilions at Arrowhead</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Dumpster</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4 YD</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2x/week</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Springs at Alta Mesa</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dumpster</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6 YD</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3x/week</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Springs at Alta Mesa</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dumpster</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4 YD</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3x/week</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Springs at Alta Mesa</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Cart</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>90 gallon</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>3x/week</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Springs at Alta Mesa</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bulk Service</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Weekly (Thursday)</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tempe Vista</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Dumpster (FEL)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4 YD</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1x/week</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Tempe Vista</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Dumpster (FEL)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3 YD</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3x/week</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tempe Vista</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Dumpster (FEL)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4 YD</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3x/week</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Club at Millenia</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Compactor</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>30 YD</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>On-call (varies)</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -71289,7 +71373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
@@ -71908,7 +71992,6 @@
         </is>
       </c>
     </row>
-    <row r="12"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -72020,19 +72103,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Yes (per T&amp;C)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>90 days (review needed)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>131941 The club at millenia_05252021113150 (2) (1).pdf</t>
@@ -72040,7 +72123,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Review Needed - May be Expired</t>
+          <t>Expired - Needs Review</t>
         </is>
       </c>
     </row>
@@ -72057,7 +72140,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>04/20/2020</t>
+          <t>04/01/2020</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -72067,24 +72150,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>04/20/2023</t>
+          <t>04/01/2023</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>Yes - 12 month terms</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>90 days (min), 180 days (max)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>Bella Mirage Waste Mgmt Contract 4.20 for 3 yrs.pdf</t>
@@ -72092,14 +72175,14 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Review Needed - May be Expired</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Orion Prosper Lakes (Little Elm)</t>
+          <t>Orion Prosper Lakes</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -72114,29 +72197,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
           <t>Little Elm 01-01-25 contract.pdf</t>
@@ -72144,7 +72227,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Active - Review for Terms</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
@@ -72161,42 +72244,42 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>McKinney Frontier Trash Agreement.pdf</t>
+          <t>McKinney Frontier Trash  Agreement.pdf</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Review Needed</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
@@ -72208,39 +72291,39 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Waste Consolidators Inc (Bulk)</t>
+          <t>Waste Consolidators Inc (Ally Waste)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>TBD - Review Bulk Contract</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I6" t="inlineStr">
         <is>
           <t>Pavilions at Arrowhead - Waste Consolidators Inc Bulk Agreement.pdf</t>
@@ -72248,7 +72331,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Review Needed</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
@@ -72260,39 +72343,39 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Waste Consolidators Inc (Bulk)</t>
+          <t>Waste Consolidators Inc (Ally Waste)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>TBD - Review Bulk Contract</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>Springs at Alta Mesa - WCI Bulk Agreement.pdf</t>
@@ -72300,7 +72383,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Review Needed</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
@@ -72312,47 +72395,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Waste Management</t>
+          <t>Waste Consolidators Inc (Ally Waste)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>01/12/2018</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TBD - Review Contract</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>TBD</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>TBD - Review Contract</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Tempe Vista - Waste Management Agreement.pdf</t>
+          <t>Tempe Vista - WCI Bulk Agreement.pdf</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Review Needed</t>
+          <t>Active - Contract on File</t>
         </is>
       </c>
     </row>
@@ -72364,7 +72447,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Republic Services</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -72404,7 +72487,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Contract Needed</t>
+          <t>Active - Contract Needed</t>
         </is>
       </c>
     </row>
@@ -72416,7 +72499,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Community Waste Disposal, LP</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -72456,7 +72539,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Contract Needed</t>
+          <t>Active - Contract Needed</t>
         </is>
       </c>
     </row>
@@ -72468,7 +72551,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Waste Management + Ally Waste</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -72508,7 +72591,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Contract Needed</t>
+          <t>Active - Contract Needed</t>
         </is>
       </c>
     </row>

</xml_diff>